<commit_message>
Correct omitted region in wage regressions
-These regressions omit South East instead of typical London
</commit_message>
<xml_diff>
--- a/input/reg_employmentSelection.xlsx
+++ b/input/reg_employmentSelection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\labsim\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A596700-A7E4-4FFF-B63D-8125BF7E54EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CE08EE-E004-469C-A109-BA13255D3331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="989" activeTab="4" xr2:uid="{B135D85C-193D-48EA-91AE-19E75650EBBD}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="83">
   <si>
     <t>REGRESSOR</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>Deh_c3_Low_Dag</t>
+  </si>
+  <si>
+    <t>UKI</t>
   </si>
 </sst>
 </file>
@@ -681,14 +684,14 @@
       <selection activeCell="A2" sqref="A2:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -700,7 +703,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -710,7 +713,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -718,7 +721,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -726,7 +729,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -734,7 +737,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -742,7 +745,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -750,7 +753,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -758,7 +761,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -784,12 +787,12 @@
       <selection activeCell="D44" sqref="D44:D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
@@ -809,7 +812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -835,7 +838,7 @@
         <v>5.7646451527085717E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -861,7 +864,7 @@
         <v>-3.8174889274016706E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -887,7 +890,7 @@
         <v>-0.48650213512349244</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -913,7 +916,7 @@
         <v>-0.33333776230736689</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -939,7 +942,7 @@
         <v>-6.811767779876339E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -965,7 +968,7 @@
         <v>-7.2922155022772273E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -991,7 +994,7 @@
         <v>-0.10655294047807748</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1017,7 +1020,7 @@
         <v>-3.5145844863158429E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1043,7 +1046,7 @@
         <v>-3.215027190546485E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>1.1879669274795224E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>-4.7304127452986178E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1121,7 +1124,7 @@
         <v>-6.4115877879110716E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1147,7 +1150,7 @@
         <v>-0.10557239353592664</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>-8.544208088959962E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1199,7 +1202,7 @@
         <v>-0.12386971391711303</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>1.8796136463467308</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1251,7 +1254,7 @@
         <v>0.1303549436042736</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>-1.2590236657543095E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1303,7 +1306,7 @@
         <v>-0.23106621236829855</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1329,7 +1332,7 @@
         <v>-8.3581775258985996E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>0.22759230642798656</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>0.33659366189861156</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>0.28864499349943756</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1433,7 +1436,7 @@
         <v>0.26511448097659907</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>0.27791965925949791</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -1485,7 +1488,7 @@
         <v>0.32268561121866679</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -1511,7 +1514,7 @@
         <v>0.27475225665808989</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>0.48448797331549642</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>0.37854100269155955</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
@@ -1589,7 +1592,7 @@
         <v>0.29781971445464106</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>23</v>
       </c>
@@ -1615,7 +1618,7 @@
         <v>0.35622742656808559</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>9.5563091068809003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
@@ -1667,7 +1670,7 @@
         <v>0.26299840993350776</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>-0.20894807529615572</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>-0.42956243305516251</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>-0.70219073659588771</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>-0.10640236440734298</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>0.64217132918305753</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>-0.32097742868980622</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -1808,14 +1811,14 @@
       <selection activeCell="D44" sqref="D44:D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.59765625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="1"/>
+    <col min="2" max="2" width="29.5703125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>3.6315342939259469E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>3.090696378873711E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>-0.28470053261154693</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>-0.26039454331730227</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>0.13493054998497719</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>-3.8427499332825854E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>1.9238293715450036E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2043,7 +2046,7 @@
         <v>1.3093395686172543E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>-5.5951450507746234E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -2095,7 +2098,7 @@
         <v>7.7024247861344819E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>0.14583800840782019</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -2147,7 +2150,7 @@
         <v>-4.135787135590123E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -2173,7 +2176,7 @@
         <v>-6.9108551859656669E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -2199,7 +2202,7 @@
         <v>4.0006155515069232E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2225,7 +2228,7 @@
         <v>-0.13996637044553256</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -2251,7 +2254,7 @@
         <v>3.283725771253819</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>0.1299328558080961</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -2303,7 +2306,7 @@
         <v>-1.2673704380862941E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -2329,7 +2332,7 @@
         <v>-0.16501807252904052</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -2355,7 +2358,7 @@
         <v>-7.7334219481094105E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>-0.10160383789821809</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>0.17828253643193698</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -2433,7 +2436,7 @@
         <v>0.11737792688148418</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>0.23153641209151987</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -2485,7 +2488,7 @@
         <v>0.23933775769929344</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2511,7 +2514,7 @@
         <v>0.38983327041600557</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -2537,7 +2540,7 @@
         <v>0.24025075184609418</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -2563,7 +2566,7 @@
         <v>0.26008418397103428</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>0.21762627031788526</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
@@ -2615,7 +2618,7 @@
         <v>0.10558297885777725</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>23</v>
       </c>
@@ -2641,7 +2644,7 @@
         <v>8.6727356997200106E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
@@ -2667,7 +2670,7 @@
         <v>-0.30442470678302536</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
@@ -2693,7 +2696,7 @@
         <v>-9.1876758940049819E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
@@ -2719,7 +2722,7 @@
         <v>6.0663097578549235E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
@@ -2745,7 +2748,7 @@
         <v>0.14675349385474248</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -2771,7 +2774,7 @@
         <v>-8.0643549334122822E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
@@ -2797,7 +2800,7 @@
         <v>-0.76723334027173307</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
@@ -2805,7 +2808,7 @@
         <v>1.2045295081933425</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -2813,7 +2816,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -2834,12 +2837,12 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2952,7 +2955,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3065,7 +3068,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -3184,7 +3187,7 @@
         <v>7.0553313750463056E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3303,7 +3306,7 @@
         <v>-8.4233751492367206E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -3422,7 +3425,7 @@
         <v>-4.4791140160401751E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -3541,7 +3544,7 @@
         <v>-1.1708687357527273E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -3660,7 +3663,7 @@
         <v>7.3567147567024947E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3779,7 +3782,7 @@
         <v>2.0295008862019137E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -3898,7 +3901,7 @@
         <v>1.5165213996484481E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -4017,7 +4020,7 @@
         <v>1.1559942168007889E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -4136,7 +4139,7 @@
         <v>1.3468575231286394E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4258,7 @@
         <v>1.6673147582043656E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -4374,7 +4377,7 @@
         <v>1.5228589015743745E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -4493,7 +4496,7 @@
         <v>3.3072333138257383E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -4612,7 +4615,7 @@
         <v>2.1481424887189552E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -4731,7 +4734,7 @@
         <v>1.893591541179676E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -4850,7 +4853,7 @@
         <v>1.6321380657944155E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -4969,7 +4972,7 @@
         <v>-2.3403241447719006E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -5088,7 +5091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -5207,7 +5210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -5326,7 +5329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -5445,7 +5448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -5564,7 +5567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -5683,7 +5686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -5802,7 +5805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -5921,7 +5924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -6040,7 +6043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -6159,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -6278,7 +6281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
@@ -6397,7 +6400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
@@ -6516,7 +6519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>23</v>
       </c>
@@ -6635,7 +6638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
@@ -6754,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
@@ -6873,7 +6876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
@@ -6992,7 +6995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
@@ -7111,7 +7114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -7230,7 +7233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
@@ -7349,7 +7352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
@@ -7481,12 +7484,12 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -7599,7 +7602,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
@@ -7712,7 +7715,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -7831,7 +7834,7 @@
         <v>2.4805696823932211E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -7950,7 +7953,7 @@
         <v>-3.0162850298519085E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -8069,7 +8072,7 @@
         <v>-5.5690786020967265E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -8188,7 +8191,7 @@
         <v>-2.3951083733515862E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -8307,7 +8310,7 @@
         <v>-5.1027595388302592E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -8426,7 +8429,7 @@
         <v>3.9093844021311538E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -8545,7 +8548,7 @@
         <v>-5.5431553264900541E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -8664,7 +8667,7 @@
         <v>9.0686468835602101E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -8783,7 +8786,7 @@
         <v>1.177044354638174E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -8902,7 +8905,7 @@
         <v>3.1592979200892051E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -9021,7 +9024,7 @@
         <v>1.4518531070721163E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -9140,7 +9143,7 @@
         <v>1.6119796797005041E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -9259,7 +9262,7 @@
         <v>4.311403950272526E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -9378,7 +9381,7 @@
         <v>-6.6098224694919488E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -9497,7 +9500,7 @@
         <v>-6.4188786923922406E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -9616,7 +9619,7 @@
         <v>-5.5544971636179864E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -9735,7 +9738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -9854,7 +9857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -9973,7 +9976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -10092,7 +10095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -10211,7 +10214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -10330,7 +10333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -10449,7 +10452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -10568,7 +10571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -10687,7 +10690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -10806,7 +10809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -10925,7 +10928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
@@ -11044,7 +11047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
@@ -11163,7 +11166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>23</v>
       </c>
@@ -11282,7 +11285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
@@ -11401,7 +11404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
@@ -11520,7 +11523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
@@ -11639,7 +11642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
@@ -11758,7 +11761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -11877,7 +11880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
@@ -11996,7 +11999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -12126,12 +12129,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
@@ -12151,7 +12154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -12177,7 +12180,7 @@
         <v>4.6915934479977849E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -12203,7 +12206,7 @@
         <v>-1.9222734930370296E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -12229,7 +12232,7 @@
         <v>-0.5640671639673901</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -12255,7 +12258,7 @@
         <v>-0.23327935640003725</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -12281,7 +12284,7 @@
         <v>0.12686023760449727</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -12307,7 +12310,7 @@
         <v>0.12129959223453655</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -12333,7 +12336,7 @@
         <v>-7.2911310959599199E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -12359,7 +12362,7 @@
         <v>4.0124633990183158E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -12385,7 +12388,7 @@
         <v>1.8483505140288836</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -12411,7 +12414,7 @@
         <v>0.222355467439417</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -12437,7 +12440,7 @@
         <v>-2.2662070051609777E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -12463,7 +12466,7 @@
         <v>-1.2542847176792222</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -12489,7 +12492,7 @@
         <v>-0.58588363714621716</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -12515,7 +12518,7 @@
         <v>0.16152782213294292</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -12541,7 +12544,7 @@
         <v>0.30431981954019538</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -12567,7 +12570,7 @@
         <v>-0.49532294568266505</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -12593,7 +12596,7 @@
         <v>-0.4578569578966018</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -12619,7 +12622,7 @@
         <v>0.63892824413571381</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -12645,7 +12648,7 @@
         <v>0.66637136214135051</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -12671,7 +12674,7 @@
         <v>-0.12453229237506515</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -12697,7 +12700,7 @@
         <v>8.2360112363702206E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -12723,7 +12726,7 @@
         <v>-2.619480976961392</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -12749,7 +12752,7 @@
         <v>9.936082077577349E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
@@ -12757,7 +12760,7 @@
         <v>0.56923974721727677</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -12765,7 +12768,7 @@
         <v>2.9607362665623915E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -12773,7 +12776,7 @@
         <v>0.56916988238278243</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
@@ -12792,12 +12795,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
@@ -12817,7 +12820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -12843,7 +12846,7 @@
         <v>2.1531316202402135E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -12869,7 +12872,7 @@
         <v>1.2526774776164333E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -12895,7 +12898,7 @@
         <v>-0.26979915241685204</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -12921,7 +12924,7 @@
         <v>-0.21794362147648899</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -12947,7 +12950,7 @@
         <v>0.12413340457879617</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -12973,7 +12976,7 @@
         <v>0.13001094243337696</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -12999,7 +13002,7 @@
         <v>-1.4701273609276304E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -13025,7 +13028,7 @@
         <v>2.3844585991469811E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -13051,7 +13054,7 @@
         <v>2.7186317410825565</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -13077,7 +13080,7 @@
         <v>0.16135372717910268</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -13103,7 +13106,7 @@
         <v>-1.4177851568920609E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -13129,7 +13132,7 @@
         <v>-0.66528963987080947</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -13155,7 +13158,7 @@
         <v>-0.1964802065364529</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -13181,7 +13184,7 @@
         <v>0.18889269597021136</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -13207,7 +13210,7 @@
         <v>0.36885903926174951</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -13233,7 +13236,7 @@
         <v>-0.39693062407133622</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -13259,7 +13262,7 @@
         <v>-0.46494546148415528</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -13285,7 +13288,7 @@
         <v>-0.48144487636540673</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -13311,7 +13314,7 @@
         <v>-0.22123672487048202</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -13337,7 +13340,7 @@
         <v>0.13706279648438247</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -13363,7 +13366,7 @@
         <v>0.6499397437057719</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -13389,7 +13392,7 @@
         <v>-0.34569631079408197</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -13415,7 +13418,7 @@
         <v>-0.52530067958047699</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
@@ -13423,7 +13426,7 @@
         <v>0.70815083726733563</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -13431,7 +13434,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -13439,7 +13442,7 @@
         <v>0.58166506869277523</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
@@ -13460,12 +13463,12 @@
       <selection activeCell="L14" sqref="L14:X26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -13536,7 +13539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
@@ -13607,7 +13610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -13684,7 +13687,7 @@
         <v>1.1949787753350353E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -13761,7 +13764,7 @@
         <v>-1.4678050056903316E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -13838,7 +13841,7 @@
         <v>-1.3441834933891231E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -13915,7 +13918,7 @@
         <v>-4.4658843580063065E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -13992,7 +13995,7 @@
         <v>6.3229148479652144E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -14069,7 +14072,7 @@
         <v>1.3218339642355971E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -14146,7 +14149,7 @@
         <v>-5.3068088763998501E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -14223,7 +14226,7 @@
         <v>-5.2347776433318935E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -14300,7 +14303,7 @@
         <v>-2.6028358840160994E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -14377,7 +14380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -14454,7 +14457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -14531,7 +14534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -14608,7 +14611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -14685,7 +14688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -14762,7 +14765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -14839,7 +14842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -14916,7 +14919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -14993,7 +14996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -15070,7 +15073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -15147,7 +15150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -15224,7 +15227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -15301,7 +15304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -15391,12 +15394,12 @@
       <selection activeCell="L14" sqref="L14:X26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -15467,7 +15470,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
@@ -15538,7 +15541,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -15615,7 +15618,7 @@
         <v>4.4983438237556592E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -15692,7 +15695,7 @@
         <v>-4.8583612558881747E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -15769,7 +15772,7 @@
         <v>-2.144880813205882E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -15846,7 +15849,7 @@
         <v>-4.8421268243430918E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -15923,7 +15926,7 @@
         <v>1.1377945851019839E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -16000,7 +16003,7 @@
         <v>3.7155731534451993E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -16077,7 +16080,7 @@
         <v>-1.0733213710838086E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -16154,7 +16157,7 @@
         <v>-1.3406152086593197E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -16231,7 +16234,7 @@
         <v>-1.0519517751866802E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -16308,7 +16311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -16385,7 +16388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -16462,7 +16465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -16539,7 +16542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -16616,7 +16619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -16693,7 +16696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -16770,7 +16773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -16847,7 +16850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -16924,7 +16927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -17001,7 +17004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -17078,7 +17081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -17155,7 +17158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -17232,7 +17235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -17318,15 +17321,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F25257F-F07C-4A46-8509-89E190CA7165}">
   <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1328125" customWidth="1"/>
-    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17409,7 +17414,7 @@
         <v>38</v>
       </c>
       <c r="AB1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="AC1" t="s">
         <v>40</v>
@@ -17427,7 +17432,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -17528,7 +17533,7 @@
         <v>1.1234287019207989E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -17629,7 +17634,7 @@
         <v>-1.3035035107919891E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -17730,7 +17735,7 @@
         <v>1.3342783150641293E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -17831,7 +17836,7 @@
         <v>-9.9982862518475484E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -17932,7 +17937,7 @@
         <v>-6.1567677542043748E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -18033,7 +18038,7 @@
         <v>2.0841050508210479E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -18134,7 +18139,7 @@
         <v>1.2795259987516253E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -18235,7 +18240,7 @@
         <v>-1.6709793783711297E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -18336,7 +18341,7 @@
         <v>-5.386309419996956E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -18437,7 +18442,7 @@
         <v>-6.0884497510483671E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -18538,7 +18543,7 @@
         <v>-4.5072551042069846E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -18639,7 +18644,7 @@
         <v>-4.4452660746244536E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -18740,7 +18745,7 @@
         <v>6.8231735574923757E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -18841,7 +18846,7 @@
         <v>1.976234861087999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -18942,7 +18947,7 @@
         <v>-4.2975803777323465E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -19043,7 +19048,7 @@
         <v>-5.3517033958145775E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -19144,7 +19149,7 @@
         <v>-5.6447175416766138E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -19245,7 +19250,7 @@
         <v>-5.9721693086180836E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -19346,7 +19351,7 @@
         <v>-6.0912425036196063E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -19447,7 +19452,7 @@
         <v>-1.2451628575935135E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -19548,7 +19553,7 @@
         <v>-1.3172001396751039E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -19649,7 +19654,7 @@
         <v>-1.4322578279203676E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -19750,7 +19755,7 @@
         <v>-1.1603090991443145E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -19851,7 +19856,7 @@
         <v>-1.3201945279932583E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -19952,9 +19957,9 @@
         <v>-1.4279948682650672E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B27">
         <v>-0.19843717585491788</v>
@@ -20053,7 +20058,7 @@
         <v>-1.35499920100745E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -20154,7 +20159,7 @@
         <v>-1.2537893142359363E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -20255,7 +20260,7 @@
         <v>-1.1381674120571575E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -20356,7 +20361,7 @@
         <v>-1.3543103214545479E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -20457,7 +20462,7 @@
         <v>-1.3679119711325898E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -20568,15 +20573,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B6C443-FF25-4392-950B-41CD47DBFEC0}">
   <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.3984375" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -20659,7 +20666,7 @@
         <v>38</v>
       </c>
       <c r="AB1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="AC1" t="s">
         <v>40</v>
@@ -20677,7 +20684,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -20778,7 +20785,7 @@
         <v>3.3852052787765736E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -20879,7 +20886,7 @@
         <v>-1.0355417896963112E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -20980,7 +20987,7 @@
         <v>1.0931275741554953E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -21081,7 +21088,7 @@
         <v>-7.063768667073483E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -21182,7 +21189,7 @@
         <v>-3.7057230421121252E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -21283,7 +21290,7 @@
         <v>1.5465079067270417E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -21384,7 +21391,7 @@
         <v>8.0983764236249636E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -21485,7 +21492,7 @@
         <v>-1.4268141125388198E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -21586,7 +21593,7 @@
         <v>-4.3379897472622513E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -21687,7 +21694,7 @@
         <v>-3.1458104356823141E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -21788,7 +21795,7 @@
         <v>-3.7995402764832065E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -21889,7 +21896,7 @@
         <v>-3.3664405517180119E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -21990,7 +21997,7 @@
         <v>3.5243833243690787E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -22091,7 +22098,7 @@
         <v>1.8773818263787363E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -22192,7 +22199,7 @@
         <v>1.5277721539412795E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -22293,7 +22300,7 @@
         <v>-3.381845591291083E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -22394,7 +22401,7 @@
         <v>-3.7310565249312894E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -22495,7 +22502,7 @@
         <v>-3.8783129830796655E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -22596,7 +22603,7 @@
         <v>-3.8775557041912838E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -22697,7 +22704,7 @@
         <v>-8.3475196992333002E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -22798,7 +22805,7 @@
         <v>-9.1197161025272425E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -22899,7 +22906,7 @@
         <v>-1.0033266847821781E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -23000,7 +23007,7 @@
         <v>-8.2702344885742863E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -23101,7 +23108,7 @@
         <v>-9.3271160070711146E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -23202,9 +23209,9 @@
         <v>-8.0980198999534001E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B27">
         <v>-0.10592557976994363</v>
@@ -23303,7 +23310,7 @@
         <v>-8.2674972482060457E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -23404,7 +23411,7 @@
         <v>-7.8710764930760323E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -23505,7 +23512,7 @@
         <v>-8.2002684001741095E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -23606,7 +23613,7 @@
         <v>-8.6218642659658448E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -23707,7 +23714,7 @@
         <v>-8.2486594915927173E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -23817,15 +23824,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0D88CC-0A74-41FF-B141-E336F245875E}">
   <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1328125" customWidth="1"/>
-    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -23905,7 +23914,7 @@
         <v>38</v>
       </c>
       <c r="AA1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="AB1" t="s">
         <v>40</v>
@@ -23923,7 +23932,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -24021,7 +24030,7 @@
         <v>-9.4189704167335522E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -24119,7 +24128,7 @@
         <v>9.6982642548876398E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -24217,7 +24226,7 @@
         <v>-6.5886249059968535E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -24315,7 +24324,7 @@
         <v>-2.9416934539061761E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -24413,7 +24422,7 @@
         <v>1.3869176160568014E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -24511,7 +24520,7 @@
         <v>6.2914050523441999E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -24609,7 +24618,7 @@
         <v>-2.7743066162202561E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -24707,7 +24716,7 @@
         <v>-4.1037595983149623E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -24805,7 +24814,7 @@
         <v>-4.8000390168310677E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -24903,7 +24912,7 @@
         <v>-3.2273352875835753E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -25001,7 +25010,7 @@
         <v>-3.5227355929362845E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -25099,7 +25108,7 @@
         <v>2.9596575798063646E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -25197,7 +25206,7 @@
         <v>1.0766787410932482E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -25295,7 +25304,7 @@
         <v>-3.0673166987609949E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -25393,7 +25402,7 @@
         <v>-6.2899460052942479E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -25491,7 +25500,7 @@
         <v>-6.3627463226519111E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -25589,7 +25598,7 @@
         <v>-6.5072148435478564E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -25687,7 +25696,7 @@
         <v>-6.6000848631958898E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -25785,7 +25794,7 @@
         <v>-6.8790020596342706E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -25883,7 +25892,7 @@
         <v>-6.4596097114570043E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -25981,7 +25990,7 @@
         <v>-6.4580699793473405E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -26079,7 +26088,7 @@
         <v>-6.2605861363566689E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -26177,7 +26186,7 @@
         <v>-7.0710243919274059E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -26275,9 +26284,9 @@
         <v>-7.2651263561485514E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B26">
         <v>-0.14923358664859429</v>
@@ -26373,7 +26382,7 @@
         <v>-7.750068431076261E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -26471,7 +26480,7 @@
         <v>-6.2559724792878859E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -26569,7 +26578,7 @@
         <v>-6.6484253095207908E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -26667,7 +26676,7 @@
         <v>-6.9323543403966201E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -26765,7 +26774,7 @@
         <v>-6.3311955163591871E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -26872,15 +26881,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055492C1-22B7-4AC3-9503-739E469FA134}">
   <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.3984375" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -26960,7 +26971,7 @@
         <v>38</v>
       </c>
       <c r="AA1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="AB1" t="s">
         <v>40</v>
@@ -26978,7 +26989,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -27076,7 +27087,7 @@
         <v>-8.015282885778125E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -27174,7 +27185,7 @@
         <v>8.6675933083272644E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -27272,7 +27283,7 @@
         <v>-4.48286561345287E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -27370,7 +27381,7 @@
         <v>-7.2651276314231834E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -27468,7 +27479,7 @@
         <v>9.5056737615150402E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -27566,7 +27577,7 @@
         <v>1.9095864061799191E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -27664,7 +27675,7 @@
         <v>-2.0252344777526759E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -27762,7 +27773,7 @@
         <v>-2.4935858210588382E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -27860,7 +27871,7 @@
         <v>-2.4639833554687191E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -27958,7 +27969,7 @@
         <v>-3.7649146693097756E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -28056,7 +28067,7 @@
         <v>-3.3306900344939742E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -28154,7 +28165,7 @@
         <v>1.7687497520361335E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -28252,7 +28263,7 @@
         <v>1.2134031824345786E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -28350,7 +28361,7 @@
         <v>-1.00718860538942E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -28448,7 +28459,7 @@
         <v>-3.3213337925816467E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -28546,7 +28557,7 @@
         <v>-3.5040132199241738E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -28644,7 +28655,7 @@
         <v>-3.5821082545806704E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -28742,7 +28753,7 @@
         <v>-3.5737522103635204E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -28840,7 +28851,7 @@
         <v>-4.3886820174622988E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -28938,7 +28949,7 @@
         <v>-5.4054214118867965E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -29036,7 +29047,7 @@
         <v>-5.0316652968294354E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -29134,7 +29145,7 @@
         <v>-4.4150680193364789E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -29232,7 +29243,7 @@
         <v>-5.2678647015680521E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -29330,9 +29341,9 @@
         <v>-5.1957979422758707E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B26">
         <v>-7.5293422121066225E-2</v>
@@ -29428,7 +29439,7 @@
         <v>-5.7823393601606483E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -29526,7 +29537,7 @@
         <v>-4.9237859464892832E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -29624,7 +29635,7 @@
         <v>-5.9367935221250054E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -29722,7 +29733,7 @@
         <v>-5.0807646941550873E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -29820,7 +29831,7 @@
         <v>-5.1042323227132487E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -29931,13 +29942,13 @@
       <selection activeCell="A6" sqref="A6:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1328125" customWidth="1"/>
-    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -30005,7 +30016,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -30073,7 +30084,7 @@
         <v>-1.3894805004880193E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -30141,7 +30152,7 @@
         <v>1.5047078714696484E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -30209,7 +30220,7 @@
         <v>-1.7136567277726774E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -30277,7 +30288,7 @@
         <v>-1.1630106780999214E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -30345,7 +30356,7 @@
         <v>-2.665007630987828E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -30413,7 +30424,7 @@
         <v>-2.7059547666375239E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -30481,7 +30492,7 @@
         <v>-2.6275528797657672E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -30549,7 +30560,7 @@
         <v>-2.6943372526787774E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -30617,7 +30628,7 @@
         <v>-2.7109855829806433E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -30685,7 +30696,7 @@
         <v>-2.6575999609536084E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -30753,7 +30764,7 @@
         <v>-2.8428697912970691E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -30821,7 +30832,7 @@
         <v>-2.7744324481718736E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -30889,7 +30900,7 @@
         <v>-2.6596784842934352E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -30957,7 +30968,7 @@
         <v>-2.4599295621478986E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -31025,7 +31036,7 @@
         <v>-2.635965748438674E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -31093,7 +31104,7 @@
         <v>-2.5624619628529721E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -31161,7 +31172,7 @@
         <v>-3.7705272835605381E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -31229,7 +31240,7 @@
         <v>7.0555345684731989E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -31297,7 +31308,7 @@
         <v>-1.0680747384473851E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -31376,13 +31387,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.3984375" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -31450,7 +31461,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -31518,7 +31529,7 @@
         <v>-1.3387946209719593E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -31586,7 +31597,7 @@
         <v>1.4843336352166981E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -31654,7 +31665,7 @@
         <v>-1.3378308948308799E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -31722,7 +31733,7 @@
         <v>-7.9254438627675207E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -31790,7 +31801,7 @@
         <v>-1.818186534766353E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -31858,7 +31869,7 @@
         <v>-1.6964089542573512E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -31926,7 +31937,7 @@
         <v>-1.9937268864974743E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -31994,7 +32005,7 @@
         <v>-1.7401169065691107E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -32062,7 +32073,7 @@
         <v>-1.8250213145314246E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -32130,7 +32141,7 @@
         <v>-1.8177900271159619E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -32198,7 +32209,7 @@
         <v>-1.9426360664431246E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -32266,7 +32277,7 @@
         <v>-1.9798687641100791E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -32334,7 +32345,7 @@
         <v>-1.7995311248620537E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -32402,7 +32413,7 @@
         <v>-1.7731894752483596E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -32470,7 +32481,7 @@
         <v>-1.7938185568325826E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -32538,7 +32549,7 @@
         <v>-2.2463037083245365E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -32606,7 +32617,7 @@
         <v>-8.4647275723906455E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -32674,7 +32685,7 @@
         <v>5.9407912715229712E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -32742,7 +32753,7 @@
         <v>-1.5178388465696751E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -32821,13 +32832,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1328125" customWidth="1"/>
-    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -32874,7 +32885,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -32921,7 +32932,7 @@
         <v>-1.8189303113043819E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -32968,7 +32979,7 @@
         <v>1.9643854106767681E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -33015,7 +33026,7 @@
         <v>-3.8733589365640446E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -33062,7 +33073,7 @@
         <v>-3.4000895646828454E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -33109,7 +33120,7 @@
         <v>-1.7611847197583654E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -33156,7 +33167,7 @@
         <v>-1.7955133573073468E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -33203,7 +33214,7 @@
         <v>-1.8697342283529187E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -33250,7 +33261,7 @@
         <v>-1.6411180807670638E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -33297,7 +33308,7 @@
         <v>-3.3126173915095708E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -33344,7 +33355,7 @@
         <v>-8.4426225226813284E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -33391,7 +33402,7 @@
         <v>7.0059316316716663E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -33438,7 +33449,7 @@
         <v>-9.5911092821069016E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -33496,13 +33507,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1328125" customWidth="1"/>
-    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -33549,7 +33560,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -33596,7 +33607,7 @@
         <v>-1.3567229363829216E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -33643,7 +33654,7 @@
         <v>1.4019761605483926E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -33690,7 +33701,7 @@
         <v>-2.3627897366036649E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -33737,7 +33748,7 @@
         <v>-1.4220370015409355E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -33784,7 +33795,7 @@
         <v>-6.6143448310304956E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -33831,7 +33842,7 @@
         <v>-7.6251697932910585E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -33878,7 +33889,7 @@
         <v>-7.6746190219970285E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -33925,7 +33936,7 @@
         <v>-7.3380030498705173E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -33972,7 +33983,7 @@
         <v>-2.9806689547212345E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -34019,7 +34030,7 @@
         <v>-7.0843860673986813E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -34066,7 +34077,7 @@
         <v>1.8787839615887341E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -34113,7 +34124,7 @@
         <v>-1.9773390160419532E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>

</xml_diff>